<commit_message>
account.pdf generated on document index and errors or validation logic build for saleTrial.xlxs file to generate transaction from excel file
</commit_message>
<xml_diff>
--- a/public/sales_trial.xlsx
+++ b/public/sales_trial.xlsx
@@ -55,7 +55,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -171,11 +171,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -328,7 +323,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -337,7 +332,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -435,10 +434,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7:C8"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -460,26 +459,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B4" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="C4" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="D4" s="0" t="n">
         <v>6000</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
-        <v>44484</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>13000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -487,11 +478,25 @@
         <v>44484</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>44484</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D6" s="0" t="n">
         <v>8000</v>
       </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>